<commit_message>
Auto-committed on 2023/03/06 週一 17:15:59.18
</commit_message>
<xml_diff>
--- a/Program/Other/LM041_底稿_催收及呆帳戶暫收款明細表.xlsx
+++ b/Program/Other/LM041_底稿_催收及呆帳戶暫收款明細表.xlsx
@@ -9,36 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="336" windowWidth="18072" windowHeight="7320"/>
+    <workbookView xWindow="600" yWindow="340" windowWidth="18070" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="D961211M" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">D961211M!$A$2:$K$2</definedName>
-    <definedName name="_xlnm.Database">D961211M!$A$2:$J$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">D961211M!$A$2:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">D961211M!$A$2:$G$2</definedName>
+    <definedName name="_xlnm.Database">D961211M!$A$2:$G$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">D961211M!$A$2:$I$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LOCNAM</t>
   </si>
   <si>
     <t>LOCLID</t>
-  </si>
-  <si>
-    <t>LGFAMTWK</t>
-  </si>
-  <si>
-    <t>ACTFEE</t>
-  </si>
-  <si>
-    <t>INSTOT</t>
   </si>
   <si>
     <t>戶況</t>
@@ -1052,25 +1043,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,58 +1066,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E3" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K2"/>
+  <autoFilter ref="A2:G2"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>